<commit_message>
Add logic to retrieve and display aggregated 'QĐ thừa' values for teachers from session state data
</commit_message>
<xml_diff>
--- a/data_base/Bang_diem_qua_trinh_(Mau).xlsx
+++ b/data_base/Bang_diem_qua_trinh_(Mau).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A6653E-35BD-4DD0-82D2-D57F5903EFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE17B80-B3EB-4FD8-858F-6D6A9A75CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hướng dẫn" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="DSMON" sheetId="11" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Bang diem thi'!$A$1:$Y$18</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Bang diem qua trinh'!$5:$5</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'Bang diem thi'!$8:$9</definedName>
   </definedNames>
@@ -1718,44 +1717,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1783,6 +1749,111 @@
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1818,78 +1889,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2852,8 +2851,8 @@
   </sheetPr>
   <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="120" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2905,17 +2904,17 @@
       <c r="O1" s="2"/>
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
-      <c r="V1" s="139" t="s">
+      <c r="V1" s="128" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="139"/>
-      <c r="X1" s="139"/>
-      <c r="Y1" s="139"/>
-      <c r="Z1" s="139"/>
-      <c r="AA1" s="139"/>
-      <c r="AB1" s="139"/>
-      <c r="AC1" s="139"/>
-      <c r="AD1" s="139"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="128"/>
+      <c r="Y1" s="128"/>
+      <c r="Z1" s="128"/>
+      <c r="AA1" s="128"/>
+      <c r="AB1" s="128"/>
+      <c r="AC1" s="128"/>
+      <c r="AD1" s="128"/>
     </row>
     <row r="2" spans="1:30" ht="15.75">
       <c r="A2" s="7"/>
@@ -2926,14 +2925,14 @@
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="142" t="s">
+      <c r="I2" s="131" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="142"/>
-      <c r="K2" s="142"/>
-      <c r="L2" s="142"/>
-      <c r="M2" s="142"/>
-      <c r="N2" s="142"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
       <c r="O2" s="42"/>
       <c r="P2" s="6" t="s">
         <v>44</v>
@@ -2941,19 +2940,19 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="144" t="s">
+      <c r="T2" s="133" t="s">
         <v>57</v>
       </c>
-      <c r="U2" s="144"/>
-      <c r="V2" s="144"/>
-      <c r="W2" s="144"/>
-      <c r="X2" s="144"/>
-      <c r="Y2" s="144"/>
-      <c r="Z2" s="144"/>
-      <c r="AA2" s="144"/>
-      <c r="AB2" s="144"/>
-      <c r="AC2" s="144"/>
-      <c r="AD2" s="144"/>
+      <c r="U2" s="133"/>
+      <c r="V2" s="133"/>
+      <c r="W2" s="133"/>
+      <c r="X2" s="133"/>
+      <c r="Y2" s="133"/>
+      <c r="Z2" s="133"/>
+      <c r="AA2" s="133"/>
+      <c r="AB2" s="133"/>
+      <c r="AC2" s="133"/>
+      <c r="AD2" s="133"/>
     </row>
     <row r="3" spans="1:30" ht="15.75">
       <c r="C3" s="8"/>
@@ -2962,14 +2961,14 @@
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="138">
+      <c r="I3" s="127">
         <v>1</v>
       </c>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="138"/>
+      <c r="J3" s="127"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="127"/>
       <c r="O3" s="42"/>
       <c r="P3" s="6" t="s">
         <v>19</v>
@@ -2989,10 +2988,10 @@
         <v>40</v>
       </c>
       <c r="Y3" s="6"/>
-      <c r="Z3" s="143" t="s">
+      <c r="Z3" s="132" t="s">
         <v>58</v>
       </c>
-      <c r="AA3" s="143"/>
+      <c r="AA3" s="132"/>
       <c r="AB3" s="63" t="s">
         <v>67</v>
       </c>
@@ -3007,14 +3006,14 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="40"/>
-      <c r="I4" s="140" t="s">
+      <c r="I4" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="140"/>
-      <c r="K4" s="140"/>
-      <c r="L4" s="140"/>
-      <c r="M4" s="140"/>
-      <c r="N4" s="140"/>
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="129"/>
       <c r="O4" s="43"/>
       <c r="P4" s="41" t="s">
         <v>17</v>
@@ -3034,72 +3033,72 @@
         <v>20</v>
       </c>
       <c r="AA4" s="41"/>
-      <c r="AB4" s="141" t="s">
+      <c r="AB4" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="AC4" s="141"/>
-      <c r="AD4" s="141"/>
+      <c r="AC4" s="130"/>
+      <c r="AD4" s="130"/>
     </row>
     <row r="5" spans="1:30" s="4" customFormat="1" ht="35.25" customHeight="1" thickTop="1">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="127" t="s">
+      <c r="B5" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="127" t="s">
+      <c r="C5" s="136" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="127"/>
-      <c r="E5" s="129" t="s">
+      <c r="D5" s="136"/>
+      <c r="E5" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="136" t="s">
+      <c r="F5" s="145" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="136"/>
-      <c r="H5" s="136"/>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="136"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="137" t="s">
+      <c r="G5" s="145"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="145"/>
+      <c r="L5" s="145"/>
+      <c r="M5" s="145"/>
+      <c r="N5" s="145"/>
+      <c r="O5" s="145"/>
+      <c r="P5" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="137"/>
-      <c r="R5" s="137"/>
-      <c r="S5" s="136" t="s">
+      <c r="Q5" s="146"/>
+      <c r="R5" s="146"/>
+      <c r="S5" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="136"/>
-      <c r="U5" s="136"/>
-      <c r="V5" s="136"/>
-      <c r="W5" s="136"/>
-      <c r="X5" s="136"/>
-      <c r="Y5" s="134" t="s">
+      <c r="T5" s="145"/>
+      <c r="U5" s="145"/>
+      <c r="V5" s="145"/>
+      <c r="W5" s="145"/>
+      <c r="X5" s="145"/>
+      <c r="Y5" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="Z5" s="133" t="s">
+      <c r="Z5" s="142" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="133"/>
-      <c r="AB5" s="133" t="s">
+      <c r="AA5" s="142"/>
+      <c r="AB5" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="AC5" s="133"/>
-      <c r="AD5" s="131" t="s">
+      <c r="AC5" s="142"/>
+      <c r="AD5" s="140" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="4" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A6" s="126"/>
-      <c r="B6" s="128"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="130"/>
+      <c r="A6" s="135"/>
+      <c r="B6" s="137"/>
+      <c r="C6" s="137"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="139"/>
       <c r="F6" s="94"/>
       <c r="G6" s="94"/>
       <c r="H6" s="94"/>
@@ -3137,7 +3136,7 @@
       <c r="X6" s="95">
         <v>6</v>
       </c>
-      <c r="Y6" s="135"/>
+      <c r="Y6" s="144"/>
       <c r="Z6" s="93" t="s">
         <v>15</v>
       </c>
@@ -3150,7 +3149,7 @@
       <c r="AC6" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="132"/>
+      <c r="AD6" s="141"/>
     </row>
     <row r="7" spans="1:30" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="80"/>
@@ -3469,13 +3468,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="V1:AD1"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="T2:AD2"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:D6"/>
@@ -3487,6 +3479,13 @@
     <mergeCell ref="S5:X5"/>
     <mergeCell ref="P5:R5"/>
     <mergeCell ref="F5:O5"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="T2:AD2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="P7:AC11">
@@ -3519,8 +3518,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="120" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3573,30 +3572,30 @@
       <c r="A2" s="5"/>
       <c r="B2" s="32"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="159" t="s">
+      <c r="D2" s="149" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="159"/>
-      <c r="F2" s="159"/>
-      <c r="G2" s="159"/>
-      <c r="H2" s="159"/>
-      <c r="I2" s="159"/>
-      <c r="J2" s="159"/>
-      <c r="K2" s="159"/>
-      <c r="L2" s="159"/>
-      <c r="M2" s="159"/>
-      <c r="N2" s="159"/>
-      <c r="O2" s="159"/>
-      <c r="P2" s="159"/>
-      <c r="Q2" s="159"/>
-      <c r="R2" s="159"/>
-      <c r="S2" s="159"/>
-      <c r="T2" s="159"/>
-      <c r="U2" s="159"/>
-      <c r="V2" s="159"/>
-      <c r="W2" s="159"/>
-      <c r="X2" s="159"/>
-      <c r="Y2" s="159"/>
+      <c r="E2" s="149"/>
+      <c r="F2" s="149"/>
+      <c r="G2" s="149"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
+      <c r="K2" s="149"/>
+      <c r="L2" s="149"/>
+      <c r="M2" s="149"/>
+      <c r="N2" s="149"/>
+      <c r="O2" s="149"/>
+      <c r="P2" s="149"/>
+      <c r="Q2" s="149"/>
+      <c r="R2" s="149"/>
+      <c r="S2" s="149"/>
+      <c r="T2" s="149"/>
+      <c r="U2" s="149"/>
+      <c r="V2" s="149"/>
+      <c r="W2" s="149"/>
+      <c r="X2" s="149"/>
+      <c r="Y2" s="149"/>
     </row>
     <row r="3" spans="1:25" ht="14.1" customHeight="1">
       <c r="A3" s="3"/>
@@ -3645,32 +3644,32 @@
         <v>14</v>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" s="178" t="str">
+      <c r="H4" s="168" t="str">
         <f>'Bang diem qua trinh'!V1</f>
         <v>Tin học</v>
       </c>
-      <c r="I4" s="178"/>
-      <c r="J4" s="178"/>
-      <c r="K4" s="178"/>
-      <c r="L4" s="178"/>
-      <c r="M4" s="178"/>
-      <c r="N4" s="178"/>
-      <c r="O4" s="178"/>
-      <c r="P4" s="178"/>
-      <c r="Q4" s="178"/>
+      <c r="I4" s="168"/>
+      <c r="J4" s="168"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="168"/>
+      <c r="M4" s="168"/>
+      <c r="N4" s="168"/>
+      <c r="O4" s="168"/>
+      <c r="P4" s="168"/>
+      <c r="Q4" s="168"/>
       <c r="R4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="S4" s="97"/>
-      <c r="T4" s="178" t="str">
+      <c r="T4" s="168" t="str">
         <f>'Bang diem qua trinh'!T2</f>
         <v>CẮT GỌT KIM LOẠI</v>
       </c>
-      <c r="U4" s="178"/>
-      <c r="V4" s="178"/>
-      <c r="W4" s="178"/>
-      <c r="X4" s="178"/>
-      <c r="Y4" s="178"/>
+      <c r="U4" s="168"/>
+      <c r="V4" s="168"/>
+      <c r="W4" s="168"/>
+      <c r="X4" s="168"/>
+      <c r="Y4" s="168"/>
     </row>
     <row r="5" spans="1:25" ht="14.65" customHeight="1">
       <c r="A5" s="10"/>
@@ -3703,13 +3702,13 @@
         <v>8</v>
       </c>
       <c r="S5" s="9"/>
-      <c r="T5" s="160" t="str">
+      <c r="T5" s="150" t="str">
         <f>IF(MID(C4,3,1)="C","Cao đẳng",IF(MID(C4,3,1)="T","Trung cấp",IF(MID(C4,3,1)="L","Liên thông Cao đẳng","")))</f>
         <v>Cao đẳng</v>
       </c>
-      <c r="U5" s="160"/>
-      <c r="V5" s="160"/>
-      <c r="W5" s="160"/>
+      <c r="U5" s="150"/>
+      <c r="V5" s="150"/>
+      <c r="W5" s="150"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="9"/>
     </row>
@@ -3744,15 +3743,15 @@
         <v>20</v>
       </c>
       <c r="S6" s="9"/>
-      <c r="T6" s="177" t="str">
+      <c r="T6" s="167" t="str">
         <f>'Bang diem qua trinh'!AB4</f>
         <v>Trương Văn Giản</v>
       </c>
-      <c r="U6" s="177"/>
-      <c r="V6" s="177"/>
-      <c r="W6" s="177"/>
-      <c r="X6" s="177"/>
-      <c r="Y6" s="177"/>
+      <c r="U6" s="167"/>
+      <c r="V6" s="167"/>
+      <c r="W6" s="167"/>
+      <c r="X6" s="167"/>
+      <c r="Y6" s="167"/>
     </row>
     <row r="7" spans="1:25" ht="7.5" customHeight="1" thickBot="1">
       <c r="A7" s="3"/>
@@ -3782,63 +3781,63 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" ht="24.75" customHeight="1" thickTop="1">
-      <c r="A8" s="145" t="s">
+      <c r="A8" s="169" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="147" t="s">
+      <c r="B8" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="149" t="s">
+      <c r="C8" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="150"/>
-      <c r="E8" s="153" t="s">
+      <c r="D8" s="174"/>
+      <c r="E8" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="155" t="s">
+      <c r="F8" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="161" t="s">
+      <c r="G8" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="162"/>
-      <c r="I8" s="171" t="s">
+      <c r="H8" s="152"/>
+      <c r="I8" s="161" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="172"/>
-      <c r="K8" s="173"/>
-      <c r="L8" s="174" t="s">
+      <c r="J8" s="162"/>
+      <c r="K8" s="163"/>
+      <c r="L8" s="164" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="175"/>
-      <c r="N8" s="175"/>
-      <c r="O8" s="175"/>
-      <c r="P8" s="175"/>
-      <c r="Q8" s="176"/>
-      <c r="R8" s="163" t="s">
+      <c r="M8" s="165"/>
+      <c r="N8" s="165"/>
+      <c r="O8" s="165"/>
+      <c r="P8" s="165"/>
+      <c r="Q8" s="166"/>
+      <c r="R8" s="153" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="165" t="s">
+      <c r="S8" s="155" t="s">
         <v>42</v>
       </c>
-      <c r="T8" s="166"/>
-      <c r="U8" s="167" t="s">
+      <c r="T8" s="156"/>
+      <c r="U8" s="157" t="s">
         <v>43</v>
       </c>
-      <c r="V8" s="168"/>
-      <c r="W8" s="157"/>
-      <c r="X8" s="158"/>
-      <c r="Y8" s="169" t="s">
+      <c r="V8" s="158"/>
+      <c r="W8" s="147"/>
+      <c r="X8" s="148"/>
+      <c r="Y8" s="159" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="146"/>
-      <c r="B9" s="148"/>
-      <c r="C9" s="151"/>
-      <c r="D9" s="152"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="156"/>
+      <c r="A9" s="170"/>
+      <c r="B9" s="172"/>
+      <c r="C9" s="175"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="180"/>
       <c r="G9" s="67" t="s">
         <v>15</v>
       </c>
@@ -3872,7 +3871,7 @@
       <c r="Q9" s="51">
         <v>6</v>
       </c>
-      <c r="R9" s="164"/>
+      <c r="R9" s="154"/>
       <c r="S9" s="69" t="s">
         <v>15</v>
       </c>
@@ -3887,7 +3886,7 @@
       </c>
       <c r="W9" s="72"/>
       <c r="X9" s="73"/>
-      <c r="Y9" s="170"/>
+      <c r="Y9" s="160"/>
     </row>
     <row r="10" spans="1:25" s="47" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="108" t="str">
@@ -3949,7 +3948,7 @@
         <f>IF('Bang diem qua trinh'!X7="","",'Bang diem qua trinh'!X7)</f>
         <v/>
       </c>
-      <c r="R10" s="179" t="str">
+      <c r="R10" s="125" t="str">
         <f>IF('Bang diem qua trinh'!Y7="","",'Bang diem qua trinh'!Y7)</f>
         <v/>
       </c>
@@ -4036,7 +4035,7 @@
         <f>IF('Bang diem qua trinh'!X8="","",'Bang diem qua trinh'!X8)</f>
         <v/>
       </c>
-      <c r="R11" s="180" t="str">
+      <c r="R11" s="126" t="str">
         <f>IF('Bang diem qua trinh'!Y8="","",'Bang diem qua trinh'!Y8)</f>
         <v/>
       </c>
@@ -4123,7 +4122,7 @@
         <f>IF('Bang diem qua trinh'!X9="","",'Bang diem qua trinh'!X9)</f>
         <v/>
       </c>
-      <c r="R12" s="180" t="str">
+      <c r="R12" s="126" t="str">
         <f>IF('Bang diem qua trinh'!Y9="","",'Bang diem qua trinh'!Y9)</f>
         <v/>
       </c>
@@ -4210,7 +4209,7 @@
         <f>IF('Bang diem qua trinh'!X10="","",'Bang diem qua trinh'!X10)</f>
         <v/>
       </c>
-      <c r="R13" s="180" t="str">
+      <c r="R13" s="126" t="str">
         <f>IF('Bang diem qua trinh'!Y10="","",'Bang diem qua trinh'!Y10)</f>
         <v/>
       </c>
@@ -4297,7 +4296,7 @@
         <f>IF('Bang diem qua trinh'!X11="","",'Bang diem qua trinh'!X11)</f>
         <v/>
       </c>
-      <c r="R14" s="180" t="str">
+      <c r="R14" s="126" t="str">
         <f>IF('Bang diem qua trinh'!Y11="","",'Bang diem qua trinh'!Y11)</f>
         <v/>
       </c>
@@ -4539,6 +4538,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="D2:Y2"/>
     <mergeCell ref="T5:W5"/>
@@ -4552,11 +4556,6 @@
     <mergeCell ref="T6:Y6"/>
     <mergeCell ref="H4:Q4"/>
     <mergeCell ref="T4:Y4"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="I10:V14">
     <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="lessThan">
@@ -4574,7 +4573,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.23622047244094491" bottom="0.23622047244094491" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="92" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>

<commit_message>
Add enrollment permissions and management pages for Admin and Tuyensinh roles
</commit_message>
<xml_diff>
--- a/data_base/Bang_diem_qua_trinh_(Mau).xlsx
+++ b/data_base/Bang_diem_qua_trinh_(Mau).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumik\Downloads\ke-khai-gio-day-app-master\data_base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE17B80-B3EB-4FD8-858F-6D6A9A75CF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3613BDA-D682-4BA6-B331-9AF1D756207B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hướng dẫn" sheetId="9" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="43">
+  <fonts count="42">
     <font>
       <sz val="12"/>
       <name val="Vni-times"/>
@@ -716,13 +716,6 @@
       <charset val="163"/>
     </font>
     <font>
-      <i/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
       <b/>
       <sz val="9"/>
       <name val="Arial"/>
@@ -762,7 +755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1118,21 +1111,6 @@
       </left>
       <right style="thin">
         <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
@@ -1176,21 +1154,6 @@
       <left style="thin">
         <color theme="1"/>
       </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color theme="1"/>
-      </top>
-      <bottom style="dotted">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -1374,7 +1337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1621,10 +1584,10 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1655,7 +1618,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1665,7 +1628,7 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="39" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1673,55 +1636,88 @@
     </xf>
     <xf numFmtId="49" fontId="39" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="39" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="39" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="42" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1749,43 +1745,40 @@
       <alignment horizontal="left" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1853,48 +1846,40 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="10"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2852,7 +2837,7 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="120" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2904,17 +2889,17 @@
       <c r="O1" s="2"/>
       <c r="T1" s="30"/>
       <c r="U1" s="30"/>
-      <c r="V1" s="128" t="s">
+      <c r="V1" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="W1" s="128"/>
-      <c r="X1" s="128"/>
-      <c r="Y1" s="128"/>
-      <c r="Z1" s="128"/>
-      <c r="AA1" s="128"/>
-      <c r="AB1" s="128"/>
-      <c r="AC1" s="128"/>
-      <c r="AD1" s="128"/>
+      <c r="W1" s="139"/>
+      <c r="X1" s="139"/>
+      <c r="Y1" s="139"/>
+      <c r="Z1" s="139"/>
+      <c r="AA1" s="139"/>
+      <c r="AB1" s="139"/>
+      <c r="AC1" s="139"/>
+      <c r="AD1" s="139"/>
     </row>
     <row r="2" spans="1:30" ht="15.75">
       <c r="A2" s="7"/>
@@ -2925,14 +2910,14 @@
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
-      <c r="I2" s="131" t="s">
+      <c r="I2" s="142" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="131"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="131"/>
-      <c r="M2" s="131"/>
-      <c r="N2" s="131"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
       <c r="O2" s="42"/>
       <c r="P2" s="6" t="s">
         <v>44</v>
@@ -2940,19 +2925,19 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-      <c r="T2" s="133" t="s">
+      <c r="T2" s="144" t="s">
         <v>57</v>
       </c>
-      <c r="U2" s="133"/>
-      <c r="V2" s="133"/>
-      <c r="W2" s="133"/>
-      <c r="X2" s="133"/>
-      <c r="Y2" s="133"/>
-      <c r="Z2" s="133"/>
-      <c r="AA2" s="133"/>
-      <c r="AB2" s="133"/>
-      <c r="AC2" s="133"/>
-      <c r="AD2" s="133"/>
+      <c r="U2" s="144"/>
+      <c r="V2" s="144"/>
+      <c r="W2" s="144"/>
+      <c r="X2" s="144"/>
+      <c r="Y2" s="144"/>
+      <c r="Z2" s="144"/>
+      <c r="AA2" s="144"/>
+      <c r="AB2" s="144"/>
+      <c r="AC2" s="144"/>
+      <c r="AD2" s="144"/>
     </row>
     <row r="3" spans="1:30" ht="15.75">
       <c r="C3" s="8"/>
@@ -2961,14 +2946,14 @@
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="127">
+      <c r="I3" s="138">
         <v>1</v>
       </c>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="138"/>
       <c r="O3" s="42"/>
       <c r="P3" s="6" t="s">
         <v>19</v>
@@ -2988,10 +2973,10 @@
         <v>40</v>
       </c>
       <c r="Y3" s="6"/>
-      <c r="Z3" s="132" t="s">
+      <c r="Z3" s="143" t="s">
         <v>58</v>
       </c>
-      <c r="AA3" s="132"/>
+      <c r="AA3" s="143"/>
       <c r="AB3" s="63" t="s">
         <v>67</v>
       </c>
@@ -3006,14 +2991,14 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="40"/>
-      <c r="I4" s="129" t="s">
+      <c r="I4" s="140" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="129"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="N4" s="129"/>
+      <c r="J4" s="140"/>
+      <c r="K4" s="140"/>
+      <c r="L4" s="140"/>
+      <c r="M4" s="140"/>
+      <c r="N4" s="140"/>
       <c r="O4" s="43"/>
       <c r="P4" s="41" t="s">
         <v>17</v>
@@ -3033,72 +3018,72 @@
         <v>20</v>
       </c>
       <c r="AA4" s="41"/>
-      <c r="AB4" s="130" t="s">
+      <c r="AB4" s="141" t="s">
         <v>21</v>
       </c>
-      <c r="AC4" s="130"/>
-      <c r="AD4" s="130"/>
+      <c r="AC4" s="141"/>
+      <c r="AD4" s="141"/>
     </row>
     <row r="5" spans="1:30" s="4" customFormat="1" ht="35.25" customHeight="1" thickTop="1">
-      <c r="A5" s="134" t="s">
+      <c r="A5" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="127" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="127" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="136"/>
-      <c r="E5" s="138" t="s">
+      <c r="D5" s="127"/>
+      <c r="E5" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="145" t="s">
+      <c r="F5" s="136" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="145"/>
-      <c r="H5" s="145"/>
-      <c r="I5" s="145"/>
-      <c r="J5" s="145"/>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146" t="s">
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="136"/>
+      <c r="L5" s="136"/>
+      <c r="M5" s="136"/>
+      <c r="N5" s="136"/>
+      <c r="O5" s="136"/>
+      <c r="P5" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="146"/>
-      <c r="R5" s="146"/>
-      <c r="S5" s="145" t="s">
+      <c r="Q5" s="137"/>
+      <c r="R5" s="137"/>
+      <c r="S5" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="T5" s="145"/>
-      <c r="U5" s="145"/>
-      <c r="V5" s="145"/>
-      <c r="W5" s="145"/>
-      <c r="X5" s="145"/>
-      <c r="Y5" s="143" t="s">
+      <c r="T5" s="136"/>
+      <c r="U5" s="136"/>
+      <c r="V5" s="136"/>
+      <c r="W5" s="136"/>
+      <c r="X5" s="136"/>
+      <c r="Y5" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="Z5" s="142" t="s">
+      <c r="Z5" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="142"/>
-      <c r="AB5" s="142" t="s">
+      <c r="AA5" s="133"/>
+      <c r="AB5" s="133" t="s">
         <v>45</v>
       </c>
-      <c r="AC5" s="142"/>
-      <c r="AD5" s="140" t="s">
+      <c r="AC5" s="133"/>
+      <c r="AD5" s="131" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:30" s="4" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A6" s="135"/>
-      <c r="B6" s="137"/>
-      <c r="C6" s="137"/>
-      <c r="D6" s="137"/>
-      <c r="E6" s="139"/>
+      <c r="A6" s="126"/>
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="130"/>
       <c r="F6" s="94"/>
       <c r="G6" s="94"/>
       <c r="H6" s="94"/>
@@ -3136,7 +3121,7 @@
       <c r="X6" s="95">
         <v>6</v>
       </c>
-      <c r="Y6" s="144"/>
+      <c r="Y6" s="135"/>
       <c r="Z6" s="93" t="s">
         <v>15</v>
       </c>
@@ -3149,7 +3134,7 @@
       <c r="AC6" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="AD6" s="141"/>
+      <c r="AD6" s="132"/>
     </row>
     <row r="7" spans="1:30" s="40" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="80"/>
@@ -3468,6 +3453,13 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="I4:N4"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="T2:AD2"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:D6"/>
@@ -3479,17 +3471,10 @@
     <mergeCell ref="S5:X5"/>
     <mergeCell ref="P5:R5"/>
     <mergeCell ref="F5:O5"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="V1:AD1"/>
-    <mergeCell ref="I4:N4"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="T2:AD2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="P7:AC11">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="lessThan">
       <formula>4.95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3519,7 +3504,7 @@
   <dimension ref="A1:Y21"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="120" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3572,30 +3557,30 @@
       <c r="A2" s="5"/>
       <c r="B2" s="32"/>
       <c r="C2" s="7"/>
-      <c r="D2" s="149" t="s">
+      <c r="D2" s="159" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="149"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="149"/>
-      <c r="H2" s="149"/>
-      <c r="I2" s="149"/>
-      <c r="J2" s="149"/>
-      <c r="K2" s="149"/>
-      <c r="L2" s="149"/>
-      <c r="M2" s="149"/>
-      <c r="N2" s="149"/>
-      <c r="O2" s="149"/>
-      <c r="P2" s="149"/>
-      <c r="Q2" s="149"/>
-      <c r="R2" s="149"/>
-      <c r="S2" s="149"/>
-      <c r="T2" s="149"/>
-      <c r="U2" s="149"/>
-      <c r="V2" s="149"/>
-      <c r="W2" s="149"/>
-      <c r="X2" s="149"/>
-      <c r="Y2" s="149"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
+      <c r="I2" s="159"/>
+      <c r="J2" s="159"/>
+      <c r="K2" s="159"/>
+      <c r="L2" s="159"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
+      <c r="O2" s="159"/>
+      <c r="P2" s="159"/>
+      <c r="Q2" s="159"/>
+      <c r="R2" s="159"/>
+      <c r="S2" s="159"/>
+      <c r="T2" s="159"/>
+      <c r="U2" s="159"/>
+      <c r="V2" s="159"/>
+      <c r="W2" s="159"/>
+      <c r="X2" s="159"/>
+      <c r="Y2" s="159"/>
     </row>
     <row r="3" spans="1:25" ht="14.1" customHeight="1">
       <c r="A3" s="3"/>
@@ -3644,32 +3629,32 @@
         <v>14</v>
       </c>
       <c r="G4" s="12"/>
-      <c r="H4" s="168" t="str">
+      <c r="H4" s="178" t="str">
         <f>'Bang diem qua trinh'!V1</f>
         <v>Tin học</v>
       </c>
-      <c r="I4" s="168"/>
-      <c r="J4" s="168"/>
-      <c r="K4" s="168"/>
-      <c r="L4" s="168"/>
-      <c r="M4" s="168"/>
-      <c r="N4" s="168"/>
-      <c r="O4" s="168"/>
-      <c r="P4" s="168"/>
-      <c r="Q4" s="168"/>
+      <c r="I4" s="178"/>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="178"/>
+      <c r="Q4" s="178"/>
       <c r="R4" s="9" t="s">
         <v>32</v>
       </c>
       <c r="S4" s="97"/>
-      <c r="T4" s="168" t="str">
+      <c r="T4" s="178" t="str">
         <f>'Bang diem qua trinh'!T2</f>
         <v>CẮT GỌT KIM LOẠI</v>
       </c>
-      <c r="U4" s="168"/>
-      <c r="V4" s="168"/>
-      <c r="W4" s="168"/>
-      <c r="X4" s="168"/>
-      <c r="Y4" s="168"/>
+      <c r="U4" s="178"/>
+      <c r="V4" s="178"/>
+      <c r="W4" s="178"/>
+      <c r="X4" s="178"/>
+      <c r="Y4" s="178"/>
     </row>
     <row r="5" spans="1:25" ht="14.65" customHeight="1">
       <c r="A5" s="10"/>
@@ -3702,13 +3687,13 @@
         <v>8</v>
       </c>
       <c r="S5" s="9"/>
-      <c r="T5" s="150" t="str">
+      <c r="T5" s="160" t="str">
         <f>IF(MID(C4,3,1)="C","Cao đẳng",IF(MID(C4,3,1)="T","Trung cấp",IF(MID(C4,3,1)="L","Liên thông Cao đẳng","")))</f>
         <v>Cao đẳng</v>
       </c>
-      <c r="U5" s="150"/>
-      <c r="V5" s="150"/>
-      <c r="W5" s="150"/>
+      <c r="U5" s="160"/>
+      <c r="V5" s="160"/>
+      <c r="W5" s="160"/>
       <c r="X5" s="11"/>
       <c r="Y5" s="9"/>
     </row>
@@ -3743,15 +3728,15 @@
         <v>20</v>
       </c>
       <c r="S6" s="9"/>
-      <c r="T6" s="167" t="str">
+      <c r="T6" s="177" t="str">
         <f>'Bang diem qua trinh'!AB4</f>
         <v>Trương Văn Giản</v>
       </c>
-      <c r="U6" s="167"/>
-      <c r="V6" s="167"/>
-      <c r="W6" s="167"/>
-      <c r="X6" s="167"/>
-      <c r="Y6" s="167"/>
+      <c r="U6" s="177"/>
+      <c r="V6" s="177"/>
+      <c r="W6" s="177"/>
+      <c r="X6" s="177"/>
+      <c r="Y6" s="177"/>
     </row>
     <row r="7" spans="1:25" ht="7.5" customHeight="1" thickBot="1">
       <c r="A7" s="3"/>
@@ -3781,63 +3766,63 @@
       <c r="Y7" s="1"/>
     </row>
     <row r="8" spans="1:25" ht="24.75" customHeight="1" thickTop="1">
-      <c r="A8" s="169" t="s">
+      <c r="A8" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="171" t="s">
+      <c r="B8" s="147" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="173" t="s">
+      <c r="C8" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="174"/>
-      <c r="E8" s="177" t="s">
+      <c r="D8" s="150"/>
+      <c r="E8" s="153" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="179" t="s">
+      <c r="F8" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="151" t="s">
+      <c r="G8" s="161" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="152"/>
-      <c r="I8" s="161" t="s">
+      <c r="H8" s="162"/>
+      <c r="I8" s="171" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="162"/>
-      <c r="K8" s="163"/>
-      <c r="L8" s="164" t="s">
+      <c r="J8" s="172"/>
+      <c r="K8" s="173"/>
+      <c r="L8" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="M8" s="165"/>
-      <c r="N8" s="165"/>
-      <c r="O8" s="165"/>
-      <c r="P8" s="165"/>
-      <c r="Q8" s="166"/>
-      <c r="R8" s="153" t="s">
+      <c r="M8" s="175"/>
+      <c r="N8" s="175"/>
+      <c r="O8" s="175"/>
+      <c r="P8" s="175"/>
+      <c r="Q8" s="176"/>
+      <c r="R8" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="S8" s="155" t="s">
+      <c r="S8" s="165" t="s">
         <v>42</v>
       </c>
-      <c r="T8" s="156"/>
-      <c r="U8" s="157" t="s">
+      <c r="T8" s="166"/>
+      <c r="U8" s="167" t="s">
         <v>43</v>
       </c>
-      <c r="V8" s="158"/>
-      <c r="W8" s="147"/>
-      <c r="X8" s="148"/>
-      <c r="Y8" s="159" t="s">
+      <c r="V8" s="168"/>
+      <c r="W8" s="157"/>
+      <c r="X8" s="158"/>
+      <c r="Y8" s="169" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:25">
-      <c r="A9" s="170"/>
-      <c r="B9" s="172"/>
-      <c r="C9" s="175"/>
-      <c r="D9" s="176"/>
-      <c r="E9" s="178"/>
-      <c r="F9" s="180"/>
+      <c r="A9" s="146"/>
+      <c r="B9" s="148"/>
+      <c r="C9" s="151"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="156"/>
       <c r="G9" s="67" t="s">
         <v>15</v>
       </c>
@@ -3871,7 +3856,7 @@
       <c r="Q9" s="51">
         <v>6</v>
       </c>
-      <c r="R9" s="154"/>
+      <c r="R9" s="164"/>
       <c r="S9" s="69" t="s">
         <v>15</v>
       </c>
@@ -3886,7 +3871,7 @@
       </c>
       <c r="W9" s="72"/>
       <c r="X9" s="73"/>
-      <c r="Y9" s="160"/>
+      <c r="Y9" s="170"/>
     </row>
     <row r="10" spans="1:25" s="47" customFormat="1" ht="15" customHeight="1">
       <c r="A10" s="108" t="str">
@@ -3948,7 +3933,7 @@
         <f>IF('Bang diem qua trinh'!X7="","",'Bang diem qua trinh'!X7)</f>
         <v/>
       </c>
-      <c r="R10" s="125" t="str">
+      <c r="R10" s="123" t="str">
         <f>IF('Bang diem qua trinh'!Y7="","",'Bang diem qua trinh'!Y7)</f>
         <v/>
       </c>
@@ -3970,361 +3955,361 @@
       </c>
       <c r="W10" s="114"/>
       <c r="X10" s="114"/>
-      <c r="Y10" s="115" t="str">
-        <f>IF(R10&lt;4.95,"KĐDT L1","")</f>
+      <c r="Y10" s="113" t="str">
+        <f>IF(R10&lt;4.95,"KĐĐKDT","")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:25" s="47" customFormat="1" ht="15" customHeight="1">
-      <c r="A11" s="116" t="str">
+      <c r="A11" s="115" t="str">
         <f>IF('Bang diem qua trinh'!A8="","",'Bang diem qua trinh'!A8)</f>
         <v/>
       </c>
-      <c r="B11" s="117" t="str">
+      <c r="B11" s="116" t="str">
         <f>IF('Bang diem qua trinh'!B8="","",'Bang diem qua trinh'!B8)</f>
         <v/>
       </c>
-      <c r="C11" s="118" t="str">
+      <c r="C11" s="117" t="str">
         <f>IF('Bang diem qua trinh'!C8="","",'Bang diem qua trinh'!C8)</f>
         <v/>
       </c>
-      <c r="D11" s="119" t="str">
+      <c r="D11" s="118" t="str">
         <f>IF('Bang diem qua trinh'!D8="","",'Bang diem qua trinh'!D8)</f>
         <v/>
       </c>
-      <c r="E11" s="117" t="str">
+      <c r="E11" s="116" t="str">
         <f>IF('Bang diem qua trinh'!E8="","",'Bang diem qua trinh'!E8)</f>
         <v/>
       </c>
-      <c r="F11" s="120"/>
-      <c r="G11" s="120"/>
-      <c r="H11" s="120"/>
-      <c r="I11" s="121">
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="119"/>
+      <c r="I11" s="120">
         <f>IF('Bang diem qua trinh'!P8="","",'Bang diem qua trinh'!P8)</f>
         <v>9</v>
       </c>
-      <c r="J11" s="121" t="str">
+      <c r="J11" s="120" t="str">
         <f>IF('Bang diem qua trinh'!Q8="","",'Bang diem qua trinh'!Q8)</f>
         <v/>
       </c>
-      <c r="K11" s="121" t="str">
+      <c r="K11" s="120" t="str">
         <f>IF('Bang diem qua trinh'!R8="","",'Bang diem qua trinh'!R8)</f>
         <v/>
       </c>
-      <c r="L11" s="121">
+      <c r="L11" s="120">
         <f>IF('Bang diem qua trinh'!S8="","",'Bang diem qua trinh'!S8)</f>
         <v>9</v>
       </c>
-      <c r="M11" s="121">
+      <c r="M11" s="120">
         <f>IF('Bang diem qua trinh'!T8="","",'Bang diem qua trinh'!T8)</f>
         <v>9</v>
       </c>
-      <c r="N11" s="121">
+      <c r="N11" s="120">
         <f>IF('Bang diem qua trinh'!U8="","",'Bang diem qua trinh'!U8)</f>
         <v>9</v>
       </c>
-      <c r="O11" s="121" t="str">
+      <c r="O11" s="120" t="str">
         <f>IF('Bang diem qua trinh'!V8="","",'Bang diem qua trinh'!V8)</f>
         <v/>
       </c>
-      <c r="P11" s="121" t="str">
+      <c r="P11" s="120" t="str">
         <f>IF('Bang diem qua trinh'!W8="","",'Bang diem qua trinh'!W8)</f>
         <v/>
       </c>
-      <c r="Q11" s="121" t="str">
+      <c r="Q11" s="120" t="str">
         <f>IF('Bang diem qua trinh'!X8="","",'Bang diem qua trinh'!X8)</f>
         <v/>
       </c>
-      <c r="R11" s="126" t="str">
+      <c r="R11" s="124" t="str">
         <f>IF('Bang diem qua trinh'!Y8="","",'Bang diem qua trinh'!Y8)</f>
         <v/>
       </c>
-      <c r="S11" s="121">
+      <c r="S11" s="120">
         <f>IF('Bang diem qua trinh'!Z8="","",'Bang diem qua trinh'!Z8)</f>
         <v>9</v>
       </c>
-      <c r="T11" s="121" t="str">
+      <c r="T11" s="120" t="str">
         <f>IF('Bang diem qua trinh'!AA8="","",'Bang diem qua trinh'!AA8)</f>
         <v/>
       </c>
-      <c r="U11" s="121" t="str">
+      <c r="U11" s="120" t="str">
         <f t="shared" ref="U11" si="0">IF(OR(R11="",S11=""),"",0.4*R11+0.6*S11)</f>
         <v/>
       </c>
-      <c r="V11" s="121" t="str">
+      <c r="V11" s="120" t="str">
         <f t="shared" ref="V11" si="1">IF(T11="","",0.4*R11+0.6*T11)</f>
         <v/>
       </c>
-      <c r="W11" s="122"/>
-      <c r="X11" s="122"/>
-      <c r="Y11" s="123" t="str">
-        <f t="shared" ref="Y11" si="2">IF(R11&lt;4.95,"KĐDT L1","")</f>
+      <c r="W11" s="121"/>
+      <c r="X11" s="121"/>
+      <c r="Y11" s="120" t="str">
+        <f t="shared" ref="Y11:Y14" si="2">IF(R11&lt;4.95,"KĐĐKDT","")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:25" s="47" customFormat="1" ht="15" customHeight="1">
-      <c r="A12" s="116" t="str">
+      <c r="A12" s="115" t="str">
         <f>IF('Bang diem qua trinh'!A9="","",'Bang diem qua trinh'!A9)</f>
         <v/>
       </c>
-      <c r="B12" s="117" t="str">
+      <c r="B12" s="116" t="str">
         <f>IF('Bang diem qua trinh'!B9="","",'Bang diem qua trinh'!B9)</f>
         <v/>
       </c>
-      <c r="C12" s="118" t="str">
+      <c r="C12" s="117" t="str">
         <f>IF('Bang diem qua trinh'!C9="","",'Bang diem qua trinh'!C9)</f>
         <v/>
       </c>
-      <c r="D12" s="119" t="str">
+      <c r="D12" s="118" t="str">
         <f>IF('Bang diem qua trinh'!D9="","",'Bang diem qua trinh'!D9)</f>
         <v/>
       </c>
-      <c r="E12" s="117" t="str">
+      <c r="E12" s="116" t="str">
         <f>IF('Bang diem qua trinh'!E9="","",'Bang diem qua trinh'!E9)</f>
         <v/>
       </c>
-      <c r="F12" s="120"/>
-      <c r="G12" s="120"/>
-      <c r="H12" s="120"/>
-      <c r="I12" s="121">
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="120">
         <f>IF('Bang diem qua trinh'!P9="","",'Bang diem qua trinh'!P9)</f>
         <v>9</v>
       </c>
-      <c r="J12" s="121" t="str">
+      <c r="J12" s="120" t="str">
         <f>IF('Bang diem qua trinh'!Q9="","",'Bang diem qua trinh'!Q9)</f>
         <v/>
       </c>
-      <c r="K12" s="121" t="str">
+      <c r="K12" s="120" t="str">
         <f>IF('Bang diem qua trinh'!R9="","",'Bang diem qua trinh'!R9)</f>
         <v/>
       </c>
-      <c r="L12" s="121">
+      <c r="L12" s="120">
         <f>IF('Bang diem qua trinh'!S9="","",'Bang diem qua trinh'!S9)</f>
         <v>9</v>
       </c>
-      <c r="M12" s="121">
+      <c r="M12" s="120">
         <f>IF('Bang diem qua trinh'!T9="","",'Bang diem qua trinh'!T9)</f>
         <v>9</v>
       </c>
-      <c r="N12" s="121">
+      <c r="N12" s="120">
         <f>IF('Bang diem qua trinh'!U9="","",'Bang diem qua trinh'!U9)</f>
         <v>9</v>
       </c>
-      <c r="O12" s="121" t="str">
+      <c r="O12" s="120" t="str">
         <f>IF('Bang diem qua trinh'!V9="","",'Bang diem qua trinh'!V9)</f>
         <v/>
       </c>
-      <c r="P12" s="121" t="str">
+      <c r="P12" s="120" t="str">
         <f>IF('Bang diem qua trinh'!W9="","",'Bang diem qua trinh'!W9)</f>
         <v/>
       </c>
-      <c r="Q12" s="121" t="str">
+      <c r="Q12" s="120" t="str">
         <f>IF('Bang diem qua trinh'!X9="","",'Bang diem qua trinh'!X9)</f>
         <v/>
       </c>
-      <c r="R12" s="126" t="str">
+      <c r="R12" s="124" t="str">
         <f>IF('Bang diem qua trinh'!Y9="","",'Bang diem qua trinh'!Y9)</f>
         <v/>
       </c>
-      <c r="S12" s="121">
+      <c r="S12" s="120">
         <f>IF('Bang diem qua trinh'!Z9="","",'Bang diem qua trinh'!Z9)</f>
         <v>9</v>
       </c>
-      <c r="T12" s="121" t="str">
+      <c r="T12" s="120" t="str">
         <f>IF('Bang diem qua trinh'!AA9="","",'Bang diem qua trinh'!AA9)</f>
         <v/>
       </c>
-      <c r="U12" s="121" t="str">
+      <c r="U12" s="120" t="str">
         <f t="shared" ref="U12:U14" si="3">IF(OR(R12="",S12=""),"",0.4*R12+0.6*S12)</f>
         <v/>
       </c>
-      <c r="V12" s="121" t="str">
+      <c r="V12" s="120" t="str">
         <f t="shared" ref="V12:V14" si="4">IF(T12="","",0.4*R12+0.6*T12)</f>
         <v/>
       </c>
-      <c r="W12" s="122"/>
-      <c r="X12" s="122"/>
-      <c r="Y12" s="123" t="str">
-        <f t="shared" ref="Y12:Y14" si="5">IF(R12&lt;4.95,"KĐDT L1","")</f>
+      <c r="W12" s="121"/>
+      <c r="X12" s="121"/>
+      <c r="Y12" s="120" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:25" s="47" customFormat="1" ht="15" customHeight="1">
-      <c r="A13" s="116" t="str">
+      <c r="A13" s="115" t="str">
         <f>IF('Bang diem qua trinh'!A10="","",'Bang diem qua trinh'!A10)</f>
         <v/>
       </c>
-      <c r="B13" s="117" t="str">
+      <c r="B13" s="116" t="str">
         <f>IF('Bang diem qua trinh'!B10="","",'Bang diem qua trinh'!B10)</f>
         <v/>
       </c>
-      <c r="C13" s="118" t="str">
+      <c r="C13" s="117" t="str">
         <f>IF('Bang diem qua trinh'!C10="","",'Bang diem qua trinh'!C10)</f>
         <v/>
       </c>
-      <c r="D13" s="119" t="str">
+      <c r="D13" s="118" t="str">
         <f>IF('Bang diem qua trinh'!D10="","",'Bang diem qua trinh'!D10)</f>
         <v/>
       </c>
-      <c r="E13" s="117" t="str">
+      <c r="E13" s="116" t="str">
         <f>IF('Bang diem qua trinh'!E10="","",'Bang diem qua trinh'!E10)</f>
         <v/>
       </c>
-      <c r="F13" s="120"/>
-      <c r="G13" s="120"/>
-      <c r="H13" s="120"/>
-      <c r="I13" s="121">
+      <c r="F13" s="119"/>
+      <c r="G13" s="119"/>
+      <c r="H13" s="119"/>
+      <c r="I13" s="120">
         <f>IF('Bang diem qua trinh'!P10="","",'Bang diem qua trinh'!P10)</f>
         <v>9</v>
       </c>
-      <c r="J13" s="121" t="str">
+      <c r="J13" s="120" t="str">
         <f>IF('Bang diem qua trinh'!Q10="","",'Bang diem qua trinh'!Q10)</f>
         <v/>
       </c>
-      <c r="K13" s="121" t="str">
+      <c r="K13" s="120" t="str">
         <f>IF('Bang diem qua trinh'!R10="","",'Bang diem qua trinh'!R10)</f>
         <v/>
       </c>
-      <c r="L13" s="121">
+      <c r="L13" s="120">
         <f>IF('Bang diem qua trinh'!S10="","",'Bang diem qua trinh'!S10)</f>
         <v>9</v>
       </c>
-      <c r="M13" s="121">
+      <c r="M13" s="120">
         <f>IF('Bang diem qua trinh'!T10="","",'Bang diem qua trinh'!T10)</f>
         <v>9</v>
       </c>
-      <c r="N13" s="121">
+      <c r="N13" s="120">
         <f>IF('Bang diem qua trinh'!U10="","",'Bang diem qua trinh'!U10)</f>
         <v>9</v>
       </c>
-      <c r="O13" s="121" t="str">
+      <c r="O13" s="120" t="str">
         <f>IF('Bang diem qua trinh'!V10="","",'Bang diem qua trinh'!V10)</f>
         <v/>
       </c>
-      <c r="P13" s="121" t="str">
+      <c r="P13" s="120" t="str">
         <f>IF('Bang diem qua trinh'!W10="","",'Bang diem qua trinh'!W10)</f>
         <v/>
       </c>
-      <c r="Q13" s="121" t="str">
+      <c r="Q13" s="120" t="str">
         <f>IF('Bang diem qua trinh'!X10="","",'Bang diem qua trinh'!X10)</f>
         <v/>
       </c>
-      <c r="R13" s="126" t="str">
+      <c r="R13" s="124" t="str">
         <f>IF('Bang diem qua trinh'!Y10="","",'Bang diem qua trinh'!Y10)</f>
         <v/>
       </c>
-      <c r="S13" s="121">
+      <c r="S13" s="120">
         <f>IF('Bang diem qua trinh'!Z10="","",'Bang diem qua trinh'!Z10)</f>
         <v>9</v>
       </c>
-      <c r="T13" s="121" t="str">
+      <c r="T13" s="120" t="str">
         <f>IF('Bang diem qua trinh'!AA10="","",'Bang diem qua trinh'!AA10)</f>
         <v/>
       </c>
-      <c r="U13" s="121" t="str">
+      <c r="U13" s="120" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V13" s="121" t="str">
+      <c r="V13" s="120" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W13" s="122"/>
-      <c r="X13" s="122"/>
-      <c r="Y13" s="123" t="str">
-        <f t="shared" si="5"/>
+      <c r="W13" s="121"/>
+      <c r="X13" s="121"/>
+      <c r="Y13" s="120" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:25" s="47" customFormat="1" ht="15" customHeight="1">
-      <c r="A14" s="116" t="str">
+      <c r="A14" s="115" t="str">
         <f>IF('Bang diem qua trinh'!A11="","",'Bang diem qua trinh'!A11)</f>
         <v/>
       </c>
-      <c r="B14" s="117" t="str">
+      <c r="B14" s="116" t="str">
         <f>IF('Bang diem qua trinh'!B11="","",'Bang diem qua trinh'!B11)</f>
         <v/>
       </c>
-      <c r="C14" s="118" t="str">
+      <c r="C14" s="117" t="str">
         <f>IF('Bang diem qua trinh'!C11="","",'Bang diem qua trinh'!C11)</f>
         <v/>
       </c>
-      <c r="D14" s="119" t="str">
+      <c r="D14" s="118" t="str">
         <f>IF('Bang diem qua trinh'!D11="","",'Bang diem qua trinh'!D11)</f>
         <v/>
       </c>
-      <c r="E14" s="117" t="str">
+      <c r="E14" s="116" t="str">
         <f>IF('Bang diem qua trinh'!E11="","",'Bang diem qua trinh'!E11)</f>
         <v/>
       </c>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="120"/>
-      <c r="I14" s="121">
+      <c r="F14" s="119"/>
+      <c r="G14" s="119"/>
+      <c r="H14" s="119"/>
+      <c r="I14" s="120">
         <f>IF('Bang diem qua trinh'!P11="","",'Bang diem qua trinh'!P11)</f>
         <v>9</v>
       </c>
-      <c r="J14" s="121" t="str">
+      <c r="J14" s="120" t="str">
         <f>IF('Bang diem qua trinh'!Q11="","",'Bang diem qua trinh'!Q11)</f>
         <v/>
       </c>
-      <c r="K14" s="121" t="str">
+      <c r="K14" s="120" t="str">
         <f>IF('Bang diem qua trinh'!R11="","",'Bang diem qua trinh'!R11)</f>
         <v/>
       </c>
-      <c r="L14" s="121">
+      <c r="L14" s="120">
         <f>IF('Bang diem qua trinh'!S11="","",'Bang diem qua trinh'!S11)</f>
         <v>9</v>
       </c>
-      <c r="M14" s="121">
+      <c r="M14" s="120">
         <f>IF('Bang diem qua trinh'!T11="","",'Bang diem qua trinh'!T11)</f>
         <v>9</v>
       </c>
-      <c r="N14" s="121">
+      <c r="N14" s="120">
         <f>IF('Bang diem qua trinh'!U11="","",'Bang diem qua trinh'!U11)</f>
         <v>9</v>
       </c>
-      <c r="O14" s="121" t="str">
+      <c r="O14" s="120" t="str">
         <f>IF('Bang diem qua trinh'!V11="","",'Bang diem qua trinh'!V11)</f>
         <v/>
       </c>
-      <c r="P14" s="121" t="str">
+      <c r="P14" s="120" t="str">
         <f>IF('Bang diem qua trinh'!W11="","",'Bang diem qua trinh'!W11)</f>
         <v/>
       </c>
-      <c r="Q14" s="121" t="str">
+      <c r="Q14" s="120" t="str">
         <f>IF('Bang diem qua trinh'!X11="","",'Bang diem qua trinh'!X11)</f>
         <v/>
       </c>
-      <c r="R14" s="126" t="str">
+      <c r="R14" s="124" t="str">
         <f>IF('Bang diem qua trinh'!Y11="","",'Bang diem qua trinh'!Y11)</f>
         <v/>
       </c>
-      <c r="S14" s="121">
+      <c r="S14" s="120">
         <f>IF('Bang diem qua trinh'!Z11="","",'Bang diem qua trinh'!Z11)</f>
         <v>9</v>
       </c>
-      <c r="T14" s="121" t="str">
+      <c r="T14" s="120" t="str">
         <f>IF('Bang diem qua trinh'!AA11="","",'Bang diem qua trinh'!AA11)</f>
         <v/>
       </c>
-      <c r="U14" s="121" t="str">
+      <c r="U14" s="120" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="V14" s="121" t="str">
+      <c r="V14" s="120" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="W14" s="122"/>
-      <c r="X14" s="122"/>
-      <c r="Y14" s="123" t="str">
-        <f t="shared" si="5"/>
+      <c r="W14" s="121"/>
+      <c r="X14" s="121"/>
+      <c r="Y14" s="113" t="str">
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:25" ht="17.25" customHeight="1">
-      <c r="A15" s="124" t="s">
+      <c r="A15" s="122" t="s">
         <v>69</v>
       </c>
       <c r="B15" s="101"/>
@@ -4538,11 +4523,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="D2:Y2"/>
     <mergeCell ref="T5:W5"/>
@@ -4556,18 +4536,43 @@
     <mergeCell ref="T6:Y6"/>
     <mergeCell ref="H4:Q4"/>
     <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="I10:V14">
-    <cfRule type="cellIs" dxfId="2" priority="6" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="lessThan">
       <formula>4.95</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W10:X14">
-    <cfRule type="cellIs" dxfId="1" priority="7" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="11" stopIfTrue="1" operator="between">
       <formula>"D"</formula>
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="8" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="12" stopIfTrue="1" operator="lessThan">
+      <formula>4.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y10:Y14">
+    <cfRule type="cellIs" dxfId="3" priority="4" stopIfTrue="1" operator="lessThan">
+      <formula>4.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y11">
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>4.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y12">
+    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="lessThan">
+      <formula>4.95</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y13">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="lessThan">
       <formula>4.95</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4579,7 +4584,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{882ABDD0-FF3F-455B-92B9-D806ED3E455F}">
+          <x14:cfRule type="expression" priority="5" id="{882ABDD0-FF3F-455B-92B9-D806ED3E455F}">
             <xm:f>'Bang diem qua trinh'!$AD7 = "Nghỉ học"</xm:f>
             <x14:dxf>
               <fill>

</xml_diff>